<commit_message>
box interval robust generation, valid inequality first iteration
</commit_message>
<xml_diff>
--- a/Data/Parabolic Trough.xlsx
+++ b/Data/Parabolic Trough.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emirsener/Desktop/Benders-Decomposition/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D3266B-E0A5-A645-B400-03F40C29E646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E07EE4-5E49-7144-AB60-2A0A326ACDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="18000" xr2:uid="{EDF38AB8-B67A-6545-84A8-C231FAB8949A}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="21680" xr2:uid="{EDF38AB8-B67A-6545-84A8-C231FAB8949A}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial values" sheetId="7" r:id="rId1"/>
@@ -513,7 +513,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -535,7 +535,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>86425338</v>
+        <v>3462184</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -559,8 +559,8 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <f>0.022*100000</f>
-        <v>2200</v>
+        <f>0.022*4020</f>
+        <v>88.44</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -585,7 +585,8 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>132000</v>
+        <f>1320 * 4.02</f>
+        <v>5306.4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -681,7 +682,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView zoomScale="161" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>